<commit_message>
code and excel update on session6, document needs changes still
</commit_message>
<xml_diff>
--- a/algstudent/Entrega 6/session6.xlsx
+++ b/algstudent/Entrega 6/session6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmene\Documents\2o\Algoritmia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmene\Documents\2o\Algoritmia\algorithmics-template\algstudent\Entrega 6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DDBD8EB-B13A-489E-8B60-060A663724A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25BE99A-D73D-4A68-B10D-0158EA405517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{F737A157-DA80-4D46-AAED-606E81387941}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Test case</t>
   </si>
@@ -74,22 +74,19 @@
     <t>Test07</t>
   </si>
   <si>
-    <t>25(LoR)</t>
-  </si>
-  <si>
     <t>2(LoR)</t>
   </si>
   <si>
-    <t>OutOfMemoryError</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>1(Lor)</t>
-  </si>
-  <si>
-    <t>7(Lor)</t>
+    <t>OOT</t>
+  </si>
+  <si>
+    <t>14(LoR)</t>
+  </si>
+  <si>
+    <t>1(LoR)</t>
   </si>
 </sst>
 </file>
@@ -111,10 +108,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFE11E46"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -149,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -157,9 +154,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A69B1366-47DC-4A55-AF9A-C58F3329AF12}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -539,13 +540,13 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2">
-        <v>64</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B3" s="3">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3">
+        <v>54</v>
+      </c>
+      <c r="D3" s="3">
         <v>12</v>
       </c>
     </row>
@@ -553,13 +554,13 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3">
         <v>1</v>
       </c>
     </row>
@@ -567,13 +568,13 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
-        <v>317</v>
-      </c>
-      <c r="C5" s="2">
-        <v>202</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B5" s="3">
+        <v>182</v>
+      </c>
+      <c r="C5" s="3">
+        <v>191</v>
+      </c>
+      <c r="D5" s="3">
         <v>3</v>
       </c>
     </row>
@@ -581,13 +582,13 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2">
-        <v>642</v>
-      </c>
-      <c r="C6" s="2">
-        <v>658</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="B6" s="3">
+        <v>213</v>
+      </c>
+      <c r="C6" s="3">
+        <v>288</v>
+      </c>
+      <c r="D6" s="3">
         <v>2</v>
       </c>
     </row>
@@ -595,13 +596,13 @@
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2">
-        <v>1964</v>
-      </c>
-      <c r="C7" s="2">
-        <v>2973</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="B7" s="3">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1253</v>
+      </c>
+      <c r="D7" s="3">
         <v>5</v>
       </c>
     </row>
@@ -609,29 +610,32 @@
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="C8" s="4">
+        <v>10435</v>
+      </c>
+      <c r="D8" s="3">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4">
+        <v>2829</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>